<commit_message>
Updated new figures to include baseline with inflation rate as control variable
</commit_message>
<xml_diff>
--- a/Output/Decomposition.xlsx
+++ b/Output/Decomposition.xlsx
@@ -56,22 +56,22 @@
   <sheetData>
     <row r="1">
       <c r="A1">
-        <v>0.80077660083770752</v>
+        <v>0.86756867170333862</v>
       </c>
       <c r="B1">
-        <v>2.2028849124908452</v>
+        <v>2.219003438949585</v>
       </c>
       <c r="C1">
-        <v>-1.2430629730224609</v>
+        <v>-1.218452930450439</v>
       </c>
       <c r="D1">
-        <v>-3.984438419342041</v>
+        <v>-4.0050206184387207</v>
       </c>
       <c r="E1">
-        <v>-2.223838329315186</v>
+        <v>-2.136902809143066</v>
       </c>
       <c r="F1">
-        <v>-682.33755252276626</v>
+        <v>-655.08083265941673</v>
       </c>
     </row>
     <row r="2">
@@ -96,202 +96,202 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>7.1019454002380371</v>
+        <v>-0.0476524047553539</v>
       </c>
       <c r="B3">
-        <v>0.50212967395782471</v>
+        <v>1.741524815559387</v>
       </c>
       <c r="C3">
-        <v>1.519248247146606</v>
+        <v>1.9635529518127439</v>
       </c>
       <c r="D3">
-        <v>-4.6041355133056641</v>
+        <v>-0.72651195526123047</v>
       </c>
       <c r="E3">
-        <v>4.5191860198974609</v>
+        <v>2.9309113025665279</v>
       </c>
       <c r="F3">
-        <v>1268.7991871211179</v>
+        <v>835.57526296724336</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>-4.5000886917114258</v>
+        <v>-4.0830531120300293</v>
       </c>
       <c r="B4">
-        <v>0.65150761604309082</v>
+        <v>0.70842981338500977</v>
       </c>
       <c r="C4">
-        <v>-2.5794823169708252</v>
+        <v>-2.4846889972686772</v>
       </c>
       <c r="D4">
-        <v>-3.1962566375732422</v>
+        <v>-3.2637290954589839</v>
       </c>
       <c r="E4">
-        <v>-9.6243181228637695</v>
+        <v>-9.123042106628418</v>
       </c>
       <c r="F4">
-        <v>-2843.3068394776592</v>
+        <v>-2680.348347935208</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>-10.23778629302979</v>
+        <v>-7.8781418800354004</v>
       </c>
       <c r="B5">
-        <v>1.529950737953186</v>
+        <v>1.4281715154647829</v>
       </c>
       <c r="C5">
-        <v>-6.2958297729492188</v>
+        <v>-6.629636287689209</v>
       </c>
       <c r="D5">
-        <v>0.98150300979614258</v>
+        <v>-1.0083484649658201</v>
       </c>
       <c r="E5">
-        <v>-14.02216625213623</v>
+        <v>-14.087953567504879</v>
       </c>
       <c r="F5">
-        <v>-4863.674397125621</v>
+        <v>-4890.2353139030411</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>3.4119632244110112</v>
+        <v>1.820960640907288</v>
       </c>
       <c r="B6">
-        <v>3.6984589099884029</v>
+        <v>3.261458158493042</v>
       </c>
       <c r="C6">
-        <v>3.776292085647583</v>
+        <v>3.1642336845397949</v>
       </c>
       <c r="D6">
-        <v>-11.624954223632811</v>
+        <v>-10.9933967590332</v>
       </c>
       <c r="E6">
-        <v>-0.7382359504699707</v>
+        <v>-2.7467401027679439</v>
       </c>
       <c r="F6">
-        <v>-153.14722714313129</v>
+        <v>-581.57982457169976</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>15.76279258728027</v>
+        <v>11.36473178863525</v>
       </c>
       <c r="B7">
-        <v>6.6526989936828613</v>
+        <v>4.3121323585510254</v>
       </c>
       <c r="C7">
-        <v>17.354976654052731</v>
+        <v>18.505096435546879</v>
       </c>
       <c r="D7">
-        <v>0.22701263427734381</v>
+        <v>4.9041824340820313</v>
       </c>
       <c r="E7">
-        <v>39.997467041015632</v>
+        <v>39.086143493652337</v>
       </c>
       <c r="F7">
-        <v>10960.79706186492</v>
+        <v>10781.242369742689</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>-15.40274047851563</v>
+        <v>-8.6794157028198242</v>
       </c>
       <c r="B8">
-        <v>-2.5303206443786621</v>
+        <v>-2.90678882598877</v>
       </c>
       <c r="C8">
-        <v>-4.7980613708496094</v>
+        <v>-5.6758871078491211</v>
       </c>
       <c r="D8">
-        <v>1.381391763687134</v>
+        <v>-1.217256546020508</v>
       </c>
       <c r="E8">
-        <v>-21.349729537963871</v>
+        <v>-18.47934722900391</v>
       </c>
       <c r="F8">
-        <v>-7350.9907776069931</v>
+        <v>-6138.6469825463982</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>-17.05447959899902</v>
+        <v>-17.688358306884769</v>
       </c>
       <c r="B9">
-        <v>4.0194416046142578</v>
+        <v>0.032858673483133302</v>
       </c>
       <c r="C9">
-        <v>-3.0640029907226558</v>
+        <v>-0.59555220603942871</v>
       </c>
       <c r="D9">
-        <v>30.073822021484379</v>
+        <v>34.269393920898438</v>
       </c>
       <c r="E9">
-        <v>13.974778175354</v>
+        <v>16.018362045288089</v>
       </c>
       <c r="F9">
-        <v>5157.1866930003771</v>
+        <v>5807.2170754401277</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>-4.2831697463989258</v>
+        <v>-4.282341480255127</v>
       </c>
       <c r="B10">
-        <v>6.0507779121398926</v>
+        <v>6.067842960357666</v>
       </c>
       <c r="C10">
-        <v>-0.26781842112541199</v>
+        <v>-0.26504403352737432</v>
       </c>
       <c r="D10">
-        <v>-0.97684288024902344</v>
+        <v>-0.98349380493164063</v>
       </c>
       <c r="E10">
-        <v>0.52294445037841797</v>
+        <v>0.5369640588760376</v>
       </c>
       <c r="F10">
-        <v>168.32799252030111</v>
+        <v>172.81659372533409</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>-9.2101449966430664</v>
+        <v>-7.4785289764404297</v>
       </c>
       <c r="B11">
-        <v>-0.091773822903633104</v>
+        <v>2.0431375503540039</v>
       </c>
       <c r="C11">
-        <v>-1.7512062788009639</v>
+        <v>-0.9100680947303772</v>
       </c>
       <c r="D11">
-        <v>-5.6691923141479492</v>
+        <v>-5.8367652893066406</v>
       </c>
       <c r="E11">
-        <v>-16.722318649291989</v>
+        <v>-12.18222141265869</v>
       </c>
       <c r="F11">
-        <v>-3706.0564789150599</v>
+        <v>-2560.2843480053721</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>-3.3514623641967769</v>
+        <v>-3.7520606517791748</v>
       </c>
       <c r="B12">
-        <v>2.210186243057251</v>
+        <v>3.2247834205627441</v>
       </c>
       <c r="C12">
-        <v>12.456562995910639</v>
+        <v>9.0975990295410156</v>
       </c>
       <c r="D12">
-        <v>-4.4639854431152344</v>
+        <v>-4.0643086433410636</v>
       </c>
       <c r="E12">
-        <v>6.8513021469116211</v>
+        <v>4.5060186386108398</v>
       </c>
       <c r="F12">
-        <v>1538.55477786249</v>
+        <v>1034.5972982684721</v>
       </c>
     </row>
   </sheetData>

</xml_diff>